<commit_message>
apac bug fix warning and image upload
</commit_message>
<xml_diff>
--- a/cass-schedule-markdown.xlsx
+++ b/cass-schedule-markdown.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassandragouldvanpraag/Library/Mobile Documents/com~apple~CloudDocs/Work/OpenSci/OHBM-OSR-2020/osr2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BADB35-D892-554B-8794-FA436806C59D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{265EBB40-E030-7845-82D5-8B9C9D8D260C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="4120" windowWidth="31520" windowHeight="21000" xr2:uid="{5936B893-C244-324D-8B60-6FA1A3F8262B}"/>
+    <workbookView xWindow="9940" yWindow="3360" windowWidth="31520" windowHeight="19440" activeTab="1" xr2:uid="{5936B893-C244-324D-8B60-6FA1A3F8262B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$N$8:$N$17</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="178">
   <si>
     <t>Privacy preserving tech: the tools for safe open data use</t>
   </si>
@@ -511,13 +513,70 @@
   </si>
   <si>
     <t>https://github.com/ohbm/osr2020/issues/59</t>
+  </si>
+  <si>
+    <t>OHBM OSR - Open Data 2.0</t>
+  </si>
+  <si>
+    <t>OHBM OSR - Open Workflows</t>
+  </si>
+  <si>
+    <t>OHBM OSR - Past, Present and Future of Open Neuroimaging</t>
+  </si>
+  <si>
+    <t>OHBM OSR - Open Science Meet Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Asia and Pacific)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Europe, Middle East and Africa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Americas)</t>
+  </si>
+  <si>
+    <t>Event joining details will be shared after registration</t>
+  </si>
+  <si>
+    <t>https://ohbm.github.io/osr2020/schedule/apac</t>
+  </si>
+  <si>
+    <t>https://ohbm.github.io/osr2020/schedule/emea</t>
+  </si>
+  <si>
+    <t>https://ohbm.github.io/osr2020/schedule/americas</t>
+  </si>
+  <si>
+    <t>Where the community thinks we are headed, what we would like to work towards and what we should be mindful of along the way.</t>
+  </si>
+  <si>
+    <t>Showcasing advances in the field of open data, collaboration and data curation.</t>
+  </si>
+  <si>
+    <t>Showcasing how we ensure individual aspects of our research workflows are transferable, reproducible and connected.</t>
+  </si>
+  <si>
+    <t>Highlights from our Hackathon, learn about elections, and ask us anything!</t>
+  </si>
+  <si>
+    <t>OHBM OSR - Open Emergent</t>
+  </si>
+  <si>
+    <t>OHBM OSR - Meet the OS-SIG</t>
+  </si>
+  <si>
+    <t>Pre-meeting welcome! Join us for informal introductions and chat with the community.</t>
+  </si>
+  <si>
+    <t>Community led discussions on any topic you'd like to offer!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -545,6 +604,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF0CAAD6"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF05323F"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -567,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -576,6 +647,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -893,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109A4615-3C85-1B4E-97AC-3FCC34413BD8}">
   <dimension ref="C4:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48:M51"/>
+    <sheetView topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2160,4 +2233,312 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EEAA2C-0311-FE46-ACFF-1E2F7AA09F56}">
+  <dimension ref="B4:D62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="59.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="4" max="4" width="82.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" t="str">
+        <f>B4&amp;C4</f>
+        <v>OHBM OSR - Open Science Meet Up (Asia and Pacific)</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" ref="D5:D31" si="0">B5&amp;C5</f>
+        <v>OHBM OSR - Open Data 2.0 (Asia and Pacific)</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Workflows (Asia and Pacific)</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Past, Present and Future of Open Neuroimaging (Asia and Pacific)</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Meet the OS-SIG (Asia and Pacific)</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Emergent (Asia and Pacific)</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Science Meet Up (Europe, Middle East and Africa)</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Data 2.0 (Europe, Middle East and Africa)</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Workflows (Europe, Middle East and Africa)</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Past, Present and Future of Open Neuroimaging (Europe, Middle East and Africa)</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Meet the OS-SIG (Europe, Middle East and Africa)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Emergent (Europe, Middle East and Africa)</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Science Meet Up (Americas)</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Data 2.0 (Americas)</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Workflows (Americas)</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Past, Present and Future of Open Neuroimaging (Americas)</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Meet the OS-SIG (Americas)</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>OHBM OSR - Open Emergent (Americas)</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" ht="20">
+      <c r="C42" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" ht="23">
+      <c r="C49" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" ht="23">
+      <c r="C52" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" ht="23">
+      <c r="C55" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C43" r:id="rId1" xr:uid="{690CE661-C2C4-C942-B86D-4EC5AC384E95}"/>
+    <hyperlink ref="C44" r:id="rId2" xr:uid="{5AD6ECA4-D674-494E-A909-39395495A82F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>